<commit_message>
updated the excel with framework related understanding
</commit_message>
<xml_diff>
--- a/Excel sheet used in class.xlsx
+++ b/Excel sheet used in class.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rames\eclipse-workspace\feb-sdet-tcs\selenium-demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E1A0824-2BF5-4392-86F0-9D72D878D755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FED9E36-F772-4C7B-9677-A64918DD4A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80FFDF1D-1FA4-4158-9897-159AD1406F2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{80FFDF1D-1FA4-4158-9897-159AD1406F2A}"/>
   </bookViews>
   <sheets>
     <sheet name="jmeter" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ide" sheetId="4" r:id="rId4"/>
     <sheet name="webdriver" sheetId="5" r:id="rId5"/>
     <sheet name="findelement &amp; findelements" sheetId="6" r:id="rId6"/>
+    <sheet name="frameworks" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="148">
   <si>
     <t>jmeter</t>
   </si>
@@ -372,13 +373,124 @@
   </si>
   <si>
     <t>if no elements gets resolved, it returns an empty list</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>webapp</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>build tools</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>testng</t>
+  </si>
+  <si>
+    <t>packages</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>pom</t>
+  </si>
+  <si>
+    <t>utils</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>test data files</t>
+  </si>
+  <si>
+    <t>configurations</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>test class</t>
+  </si>
+  <si>
+    <t>test cases</t>
+  </si>
+  <si>
+    <t>test methods</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>external source</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>SDSF</t>
+  </si>
+  <si>
+    <t>NSDSF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard </t>
+  </si>
+  <si>
+    <t>serialization</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>yaml</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>allure reports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,8 +520,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +551,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -514,12 +646,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,8 +687,21 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -566,38 +712,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126DC53B-BB96-4FDB-9287-E4DF0B19297F}">
   <dimension ref="D4:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -936,10 +1091,10 @@
       </c>
     </row>
     <row r="5" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -950,8 +1105,8 @@
       </c>
     </row>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="14">
+      <c r="D6" s="19"/>
+      <c r="E6" s="4">
         <v>2</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -960,14 +1115,14 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="4"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
-      <c r="E8" s="14">
+      <c r="D8" s="19"/>
+      <c r="E8" s="4">
         <v>3</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -976,8 +1131,8 @@
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="E9" s="14">
+      <c r="D9" s="19"/>
+      <c r="E9" s="4">
         <v>4</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -986,14 +1141,14 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="4"/>
-      <c r="E10" s="16"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="4"/>
-      <c r="E11" s="14">
+      <c r="D11" s="19"/>
+      <c r="E11" s="4">
         <v>5</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -1002,8 +1157,8 @@
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="4"/>
-      <c r="E12" s="14">
+      <c r="D12" s="19"/>
+      <c r="E12" s="4">
         <v>6</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -1012,8 +1167,8 @@
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
-      <c r="E13" s="14">
+      <c r="D13" s="19"/>
+      <c r="E13" s="4">
         <v>7</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -1022,8 +1177,8 @@
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="4"/>
-      <c r="E14" s="14">
+      <c r="D14" s="19"/>
+      <c r="E14" s="4">
         <v>8</v>
       </c>
       <c r="F14" s="9" t="s">
@@ -1034,11 +1189,11 @@
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="5"/>
-      <c r="E15" s="15">
+      <c r="D15" s="20"/>
+      <c r="E15" s="5">
         <v>9</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="9"/>
@@ -1077,14 +1232,14 @@
       <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F6" s="6" t="s">
@@ -1114,17 +1269,17 @@
       <c r="F7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
     </row>
     <row r="8" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F8" s="6" t="s">
@@ -1139,10 +1294,10 @@
       <c r="G9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="17"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F10" s="6" t="s">
@@ -1154,7 +1309,7 @@
       <c r="K10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="14">
         <v>0.8</v>
       </c>
     </row>
@@ -1175,16 +1330,16 @@
       </c>
     </row>
     <row r="13" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="17"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="7" t="s">
@@ -1198,7 +1353,7 @@
       <c r="F15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1206,111 +1361,111 @@
       <c r="F16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="17"/>
-      <c r="N16" s="17" t="s">
+      <c r="K16" s="21"/>
+      <c r="N16" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="O16" s="17"/>
+      <c r="O16" s="21"/>
     </row>
     <row r="17" spans="6:15" x14ac:dyDescent="0.25">
       <c r="J17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="22" t="s">
         <v>21</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="21"/>
       <c r="J18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="20"/>
+      <c r="K18" s="22"/>
       <c r="N18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="20"/>
+      <c r="O18" s="22"/>
     </row>
     <row r="19" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="22" t="s">
         <v>21</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="20"/>
+      <c r="K19" s="22"/>
       <c r="N19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O19" s="20"/>
+      <c r="O19" s="22"/>
     </row>
     <row r="20" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="G20" s="22"/>
       <c r="J20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="20"/>
+      <c r="K20" s="22"/>
       <c r="N20" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="O20" s="20"/>
+      <c r="O20" s="22"/>
     </row>
     <row r="21" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="20"/>
+      <c r="G21" s="22"/>
       <c r="N21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O21" s="20"/>
+      <c r="O21" s="22"/>
     </row>
     <row r="22" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="20"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="K23" s="17" t="s">
+      <c r="G23" s="22"/>
+      <c r="K23" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="L23" s="17"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="20"/>
+      <c r="G24" s="22"/>
       <c r="K24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L24" s="17" t="s">
+      <c r="L24" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1318,31 +1473,31 @@
       <c r="F25" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="20"/>
+      <c r="G25" s="22"/>
       <c r="K25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L25" s="17"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="6:15" x14ac:dyDescent="0.25">
       <c r="K26" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="L26" s="17"/>
+      <c r="L26" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="G19:G25"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="K17:K20"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="L24:L26"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="J5:O5"/>
     <mergeCell ref="J7:O7"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="G19:G25"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="K17:K20"/>
     <mergeCell ref="O17:O21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1504,7 +1659,7 @@
       </c>
     </row>
     <row r="12" spans="8:17" x14ac:dyDescent="0.25">
-      <c r="J12" s="21">
+      <c r="J12" s="15">
         <v>43405</v>
       </c>
       <c r="K12" t="s">
@@ -1570,31 +1725,31 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="18" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="18" t="s">
         <v>93</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1608,12 +1763,12 @@
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="5"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="2" t="s">
         <v>96</v>
       </c>
@@ -1690,50 +1845,392 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="57.85546875" style="25" customWidth="1"/>
+    <col min="5" max="6" width="57.85546875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="5:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="11" spans="5:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="17" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="12" spans="5:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="17" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0B605B-6EF9-4FDB-945B-74E1370F84EB}">
+  <dimension ref="B2:O25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="10" max="10" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D6" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D7" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="29"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="32"/>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="G7:G12"/>
+    <mergeCell ref="H7:H12"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="I7:I12"/>
+    <mergeCell ref="J7:J12"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C14:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>